<commit_message>
other templates rebased on master
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_extraction_vtest.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_extraction_vtest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="440">
   <si>
     <t xml:space="preserve">Nucleic Acid Extraction template</t>
   </si>
@@ -161,40 +161,61 @@
     <t xml:space="preserve">BIOPSY</t>
   </si>
   <si>
+    <t xml:space="preserve">Tube Strip 2x1</t>
+  </si>
+  <si>
     <t xml:space="preserve">A05</t>
   </si>
   <si>
     <t xml:space="preserve">BLOOD</t>
   </si>
   <si>
+    <t xml:space="preserve">Tube Strip 3x1</t>
+  </si>
+  <si>
     <t xml:space="preserve">A06</t>
   </si>
   <si>
     <t xml:space="preserve">CELLS</t>
   </si>
   <si>
+    <t xml:space="preserve">Tube Strip 4x1</t>
+  </si>
+  <si>
     <t xml:space="preserve">A07</t>
   </si>
   <si>
     <t xml:space="preserve">EXPECTORATION</t>
   </si>
   <si>
+    <t xml:space="preserve">Tube Strip 5x1</t>
+  </si>
+  <si>
     <t xml:space="preserve">A08</t>
   </si>
   <si>
     <t xml:space="preserve">GARGLE</t>
   </si>
   <si>
+    <t xml:space="preserve">Tube Strip 6x1</t>
+  </si>
+  <si>
     <t xml:space="preserve">A09</t>
   </si>
   <si>
     <t xml:space="preserve">PLASMA</t>
   </si>
   <si>
+    <t xml:space="preserve">Tube Strip 7x1</t>
+  </si>
+  <si>
     <t xml:space="preserve">A10</t>
   </si>
   <si>
     <t xml:space="preserve">SALIVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tube Strip 8x1</t>
   </si>
   <si>
     <t xml:space="preserve">A11</t>
@@ -1839,10 +1860,10 @@
   <dimension ref="A1:AE711"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.65625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16"/>
@@ -4203,12 +4224,12 @@
       <formula1>Index!$A$2:$A$97</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H9:H104" type="list">
-      <formula1>Index!$D$2:$D$4</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F9:F104" type="list">
+      <formula1>IF($H9="384-well plate",Index!$B$2:$B$385,IF($H9="96-well plate", Index!$A$2:$A$97, ""))</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F9:F104" type="list">
-      <formula1>IF($H9="384-well plate",Index!$B$2:$B$385,IF($H9="96-well plate", Index!$A$2:$A$97, ""))</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H9:H104" type="list">
+      <formula1>Index!$D$2:$D$11</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -4227,20 +4248,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G386"/>
+  <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.65625" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6484375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="9.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="8" style="0" width="9.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4335,7 +4358,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="40" t="s">
         <v>44</v>
       </c>
@@ -4345,2202 +4368,2223 @@
       <c r="C5" s="40" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="40" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>48</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="40" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>51</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="40" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C8" s="40" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>54</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="40" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>57</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="40" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>60</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="40" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>57</v>
+        <v>63</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="40" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C12" s="41" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="40" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="40" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="40" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="40" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="40" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B17" s="40" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="40" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="40" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B19" s="40" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="40" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B20" s="40" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="40" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B21" s="40" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="40" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B22" s="40" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="40" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B23" s="40" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="40" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B24" s="40" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="40" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="B25" s="40" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="40" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B26" s="40" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="40" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="40" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="B28" s="40" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="40" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B29" s="40" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="40" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B30" s="40" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="40" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B31" s="40" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="40" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="B32" s="40" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="40" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B33" s="40" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="40" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B34" s="40" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="40" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="B35" s="40" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="40" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B36" s="40" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="40" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B37" s="40" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="40" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B38" s="40" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="40" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B39" s="40" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="40" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B40" s="40" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="40" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="B41" s="40" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="40" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="B42" s="40" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="40" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="B43" s="40" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="40" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B44" s="40" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="40" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B45" s="40" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="40" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="B46" s="40" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="40" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B47" s="40" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="40" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B48" s="40" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="40" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="B49" s="40" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="40" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B50" s="40" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="40" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="B51" s="40" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="40" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="B52" s="40" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="40" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B53" s="40" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="40" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="B54" s="40" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="40" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="B55" s="40" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="40" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B56" s="40" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="40" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="B57" s="40" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="40" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="B58" s="40" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="40" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="B59" s="40" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="40" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="B60" s="40" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="40" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="B61" s="40" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="40" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="B62" s="40" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="40" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="B63" s="40" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="40" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="B64" s="40" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="40" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="B65" s="40" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="40" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="B66" s="40" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="40" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="B67" s="40" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="40" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="B68" s="40" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="40" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B69" s="40" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="40" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B70" s="40" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="40" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="B71" s="40" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="40" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="B72" s="40" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="40" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="B73" s="40" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="40" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="B74" s="40" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="40" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="B75" s="40" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="40" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="B76" s="40" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="40" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="B77" s="40" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="40" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="B78" s="40" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="40" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="B79" s="40" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="40" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="B80" s="40" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="40" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="B81" s="40" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="40" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="B82" s="40" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="40" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B83" s="40" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="40" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="B84" s="40" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="40" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="B85" s="40" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="40" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="B86" s="40" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="40" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="B87" s="40" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="40" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="B88" s="40" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="40" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B89" s="40" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="40" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="B90" s="40" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="40" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="B91" s="40" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="40" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="B92" s="40" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="40" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="B93" s="40" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="40" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="B94" s="40" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="40" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="B95" s="40" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="40" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="B96" s="40" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="40" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="B97" s="40" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B98" s="40" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B99" s="40" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B100" s="40" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B101" s="40" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B102" s="40" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B103" s="40" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B104" s="40" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B105" s="40" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B106" s="40" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B107" s="40" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B108" s="40" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B109" s="40" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B110" s="40" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B111" s="40" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B112" s="40" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B113" s="40" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B114" s="40" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B115" s="40" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B116" s="40" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B117" s="40" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B118" s="40" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B119" s="40" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B120" s="40" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B121" s="40" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B122" s="40" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B123" s="40" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B124" s="40" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B125" s="40" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B126" s="40" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B127" s="40" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B128" s="40" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B129" s="40" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B130" s="40" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B131" s="40" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B132" s="40" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B133" s="40" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B134" s="40" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B135" s="40" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B136" s="40" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B137" s="40" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B138" s="40" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B139" s="40" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B140" s="40" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B141" s="40" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B142" s="40" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B143" s="40" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B144" s="40" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B145" s="40" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B146" s="40" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B147" s="40" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B148" s="40" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B149" s="40" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B150" s="40" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B151" s="40" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B152" s="40" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B153" s="40" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B154" s="40" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B155" s="40" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B156" s="40" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B157" s="40" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B158" s="40" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B159" s="40" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B160" s="40" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B161" s="40" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B162" s="40" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B163" s="40" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B164" s="40" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B165" s="40" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B166" s="40" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B167" s="40" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B168" s="40" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B169" s="40" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B170" s="40" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B171" s="40" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B172" s="40" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B173" s="40" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B174" s="40" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B175" s="40" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B176" s="40" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B177" s="40" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B178" s="40" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B179" s="40" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B180" s="40" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B181" s="40" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B182" s="40" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B183" s="40" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B184" s="40" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B185" s="40" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B186" s="40" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B187" s="40" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B188" s="40" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B189" s="40" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B190" s="40" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B191" s="40" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B192" s="40" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B193" s="40" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B194" s="40" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B195" s="40" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B196" s="40" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B197" s="40" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B198" s="40" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B199" s="40" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B200" s="40" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B201" s="40" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B202" s="40" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B203" s="40" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B204" s="40" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B205" s="40" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B206" s="40" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B207" s="40" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B208" s="40" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B209" s="40" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B210" s="40" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B211" s="40" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B212" s="40" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B213" s="40" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B214" s="40" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B215" s="40" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B216" s="40" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B217" s="40" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B218" s="40" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B219" s="40" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B220" s="40" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B221" s="40" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B222" s="40" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B223" s="40" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B224" s="40" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B225" s="40" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B226" s="40" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B227" s="40" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B228" s="40" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B229" s="40" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B230" s="40" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B231" s="40" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B232" s="40" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B233" s="40" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B234" s="40" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B235" s="40" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B236" s="40" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B237" s="40" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B238" s="40" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B239" s="40" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B240" s="40" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B241" s="40" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B242" s="40" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B243" s="40" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B244" s="40" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B245" s="40" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B246" s="40" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B247" s="40" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B248" s="40" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B249" s="40" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B250" s="40" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B251" s="40" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B252" s="40" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B253" s="40" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B254" s="40" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B255" s="40" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B256" s="40" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B257" s="40" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B258" s="40" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B259" s="40" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B260" s="40" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B261" s="40" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B262" s="40" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B263" s="40" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B264" s="40" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B265" s="40" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B266" s="40" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B267" s="40" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B268" s="40" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B269" s="40" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B270" s="40" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B271" s="40" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B272" s="40" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B273" s="40" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B274" s="40" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B275" s="40" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B276" s="40" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B277" s="40" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B278" s="40" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B279" s="40" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B280" s="40" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B281" s="40" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B282" s="40" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B283" s="40" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B284" s="40" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B285" s="40" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B286" s="40" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B287" s="40" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B288" s="40" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B289" s="40" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B290" s="40" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B291" s="40" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B292" s="40" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B293" s="40" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B294" s="40" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B295" s="40" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B296" s="40" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B297" s="40" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B298" s="40" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B299" s="40" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B300" s="40" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B301" s="40" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B302" s="40" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B303" s="40" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B304" s="40" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B305" s="40" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B306" s="40" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B307" s="40" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B308" s="40" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B309" s="40" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B310" s="40" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B311" s="40" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B312" s="40" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B313" s="40" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B314" s="40" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B315" s="40" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B316" s="40" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B317" s="40" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B318" s="40" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B319" s="40" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B320" s="40" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B321" s="40" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B322" s="40" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B323" s="40" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B324" s="40" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B325" s="40" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B326" s="40" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B327" s="40" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B328" s="40" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B329" s="40" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B330" s="40" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B331" s="40" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B332" s="40" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B333" s="40" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B334" s="40" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B335" s="40" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B336" s="40" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B337" s="40" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B338" s="40" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B339" s="40" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B340" s="40" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B341" s="40" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B342" s="40" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B343" s="40" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B344" s="40" t="s">
-        <v>391</v>
+        <v>398</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B345" s="40" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B346" s="40" t="s">
-        <v>393</v>
+        <v>400</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B347" s="40" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B348" s="40" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B349" s="40" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B350" s="40" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B351" s="40" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B352" s="40" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B353" s="40" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B354" s="40" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B355" s="40" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B356" s="40" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B357" s="40" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B358" s="40" t="s">
-        <v>405</v>
+        <v>412</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B359" s="40" t="s">
-        <v>406</v>
+        <v>413</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B360" s="40" t="s">
-        <v>407</v>
+        <v>414</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B361" s="40" t="s">
-        <v>408</v>
+        <v>415</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B362" s="40" t="s">
-        <v>409</v>
+        <v>416</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B363" s="40" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B364" s="40" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B365" s="40" t="s">
-        <v>412</v>
+        <v>419</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B366" s="40" t="s">
-        <v>413</v>
+        <v>420</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B367" s="40" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B368" s="40" t="s">
-        <v>415</v>
+        <v>422</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B369" s="40" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B370" s="40" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B371" s="40" t="s">
-        <v>418</v>
+        <v>425</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B372" s="40" t="s">
-        <v>419</v>
+        <v>426</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B373" s="40" t="s">
-        <v>420</v>
+        <v>427</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B374" s="40" t="s">
-        <v>421</v>
+        <v>428</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B375" s="40" t="s">
-        <v>422</v>
+        <v>429</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B376" s="40" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B377" s="40" t="s">
-        <v>424</v>
+        <v>431</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B378" s="40" t="s">
-        <v>425</v>
+        <v>432</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B379" s="40" t="s">
-        <v>426</v>
+        <v>433</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B380" s="40" t="s">
-        <v>427</v>
+        <v>434</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B381" s="40" t="s">
-        <v>428</v>
+        <v>435</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B382" s="40" t="s">
-        <v>429</v>
+        <v>436</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B383" s="40" t="s">
-        <v>430</v>
+        <v>437</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B384" s="40" t="s">
-        <v>431</v>
+        <v>438</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B385" s="40" t="s">
-        <v>432</v>
+        <v>439</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>